<commit_message>
updated codes and base files
</commit_message>
<xml_diff>
--- a/project/COPPER/sample_generators/COPPER_configuration.xlsx
+++ b/project/COPPER/sample_generators/COPPER_configuration.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smoha\Documents\Git\m3_modelling\ML\COPPER\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smoha\Documents\Git\ml_progress\project\COPPER\sample_generators\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26914A9B-5998-4A50-8661-483AFFEF1A49}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{113D459B-DB81-4E2E-8EB2-307FE97A51BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -532,7 +532,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>

</xml_diff>